<commit_message>
slide animation update animation between activities update data excel update
</commit_message>
<xml_diff>
--- a/storyboard/Reinbow Defense 데이터.xlsx
+++ b/storyboard/Reinbow Defense 데이터.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HyeonMyeong\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d00rc\AndroidStudioProjects\RainbowDefense\storyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{756FE4F2-6929-4013-9A72-A8D8511CA749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA1AAA5-1732-4650-AA4B-DB0312CA0502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{500AC797-2A8F-4B60-814B-8827FBFBFF78}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{500AC797-2A8F-4B60-814B-8827FBFBFF78}"/>
   </bookViews>
   <sheets>
     <sheet name="유닛" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="75">
   <si>
     <t>Shape</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -206,6 +206,134 @@
   </si>
   <si>
     <t>애니메이션 효과</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>movespeed</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackspeed</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>redbean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>yellowbean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>greenbean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>bluebean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>indigobean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>purplebean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reward</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>info</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>strong damage</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>lot money</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>heal</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>teleport</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>hard</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>debuff</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stage</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>redjelly</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>orangejelly</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>orangebean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>yellowjelly</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>greenjelly</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>bluejelly</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>indigojelly</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>purplejelly</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>wave</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>difficulty</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -383,9 +511,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -393,6 +518,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -422,6 +550,939 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="직사각형 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE2C19D-CE32-4A06-8667-6AEAADA74852}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="873127"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="직사각형 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD750F48-64FD-4000-BDA7-E15D17DA93D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="873127"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="직사각형 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DEF3DC3-C56C-4F47-811A-E97442655C95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="873127"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="직사각형 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9AEA8A2-F533-4880-B9A1-5827BD306EC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="1890994"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="직사각형 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50EBB18B-35D1-4B06-9FAA-1DCB667551D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="1890994"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="직사각형 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D18DE722-A902-49FB-A39C-A07D4AF2911A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="1890994"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="직사각형 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0375C6F-E3EB-4ADE-BF21-1E9FE1F21B2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="1890994"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="직사각형 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A36C061-FB14-4763-802F-C45DC427AF8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="1890994"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="직사각형 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27FE4346-B526-4DDF-9CD1-ADC153ADA79D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316691" y="1890994"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="직사각형 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F206C2B-7C8D-4C6D-B68B-AE77BF73A5B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1329531" y="5580181"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="직사각형 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{975F8C2D-D253-4ADF-8BCC-41629024F0BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1329531" y="6086197"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="직사각형 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4ACC4A-532C-4B62-A9BD-0CB95707FB1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1329531" y="5580181"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="직사각형 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF4707CE-3846-4C79-B46E-F5E34BF6EC04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1329531" y="5580181"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>14009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574302</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>494927</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="직사각형 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{487D6FB5-166B-4C43-9AC5-DD2CD060F1C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1329531" y="5580181"/>
+          <a:ext cx="574302" cy="480918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -721,27 +1782,619 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CFA28D-5916-4CA2-BBEC-D5601984DC3F}">
-  <dimension ref="A1"/>
+  <dimension ref="D4:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:H4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:8">
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69F6702-DBF8-4E58-9A92-A08DBB558361}">
-  <dimension ref="A1"/>
+  <dimension ref="D4:U28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="2" width="8.6640625" style="1"/>
+    <col min="3" max="3" width="7.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.58203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.6640625" style="1"/>
+    <col min="11" max="11" width="14.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:21" ht="28.5" customHeight="1">
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="4:21" ht="40" customHeight="1">
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1">
+        <v>50</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>700</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1">
+        <v>4</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:21" ht="40" customHeight="1">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1">
+        <v>700</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N6" s="1">
+        <v>2</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T6" s="1">
+        <v>4</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:21" ht="40" customHeight="1">
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>700</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="1">
+        <v>3</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="T7" s="1">
+        <v>4</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:21" ht="40" customHeight="1">
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <v>50</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>700</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="1">
+        <v>4</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="R8" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="T8" s="1">
+        <v>4</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="4:21" ht="40" customHeight="1">
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <v>700</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>5</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="1">
+        <v>5</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="T9" s="1">
+        <v>4</v>
+      </c>
+      <c r="U9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:21" ht="40" customHeight="1">
+      <c r="D10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="1">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1">
+        <v>700</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>5</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" s="1">
+        <v>6</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="S10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="T10" s="1">
+        <v>4</v>
+      </c>
+      <c r="U10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:21" ht="40" customHeight="1">
+      <c r="D11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="1">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1">
+        <v>700</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="1">
+        <v>5</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" s="1">
+        <v>7</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="R11" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="T11" s="1">
+        <v>4</v>
+      </c>
+      <c r="U11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:21" ht="40" customHeight="1">
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="1">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1">
+        <v>700</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="1">
+        <v>5</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="4:21" ht="40" customHeight="1">
+      <c r="D13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1">
+        <v>700</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="1">
+        <v>5</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="4:21" ht="40" customHeight="1">
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="1">
+        <v>50</v>
+      </c>
+      <c r="F14" s="1">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1">
+        <v>700</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="1">
+        <v>5</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="4:21" ht="40" customHeight="1">
+      <c r="D15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="1">
+        <v>50</v>
+      </c>
+      <c r="F15" s="1">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1">
+        <v>700</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="1">
+        <v>5</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="4:21" ht="40" customHeight="1">
+      <c r="D16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1">
+        <v>50</v>
+      </c>
+      <c r="F16" s="1">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1">
+        <v>700</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="1">
+        <v>5</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" ht="40" customHeight="1">
+      <c r="D17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="1">
+        <v>50</v>
+      </c>
+      <c r="F17" s="1">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1">
+        <v>700</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J17" s="1">
+        <v>5</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" ht="40" customHeight="1">
+      <c r="D18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="1">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1">
+        <v>10</v>
+      </c>
+      <c r="G18" s="1">
+        <v>700</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J18" s="1">
+        <v>5</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" ht="40" customHeight="1"/>
+    <row r="20" spans="4:11" ht="40" customHeight="1"/>
+    <row r="21" spans="4:11" ht="40" customHeight="1"/>
+    <row r="22" spans="4:11" ht="40" customHeight="1"/>
+    <row r="23" spans="4:11" ht="40" customHeight="1"/>
+    <row r="24" spans="4:11" ht="40" customHeight="1"/>
+    <row r="25" spans="4:11" ht="40" customHeight="1"/>
+    <row r="26" spans="4:11" ht="40" customHeight="1"/>
+    <row r="27" spans="4:11" ht="40" customHeight="1"/>
+    <row r="28" spans="4:11" ht="40" customHeight="1"/>
+  </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -749,54 +2402,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2BB7B9-61DB-4CDF-9C38-75600D356E65}">
   <dimension ref="B2:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="2" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
     <col min="6" max="8" width="17.25" customWidth="1"/>
-    <col min="10" max="12" width="13.875" customWidth="1"/>
+    <col min="10" max="12" width="13.83203125" customWidth="1"/>
     <col min="14" max="16" width="16.75" customWidth="1"/>
-    <col min="18" max="20" width="14.625" customWidth="1"/>
-    <col min="22" max="24" width="14.875" customWidth="1"/>
+    <col min="18" max="20" width="14.58203125" customWidth="1"/>
+    <col min="22" max="24" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="17.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:24" ht="17.5">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="V2" s="2" t="s">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="V2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="2:24" ht="17.25">
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+    </row>
+    <row r="3" spans="2:24" ht="17.5">
       <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
@@ -829,724 +2482,724 @@
       <c r="X3" s="8"/>
     </row>
     <row r="4" spans="2:24">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="V4" s="3" t="s">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="V4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:24">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="V5" s="3" t="s">
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="V5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="W5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="X5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:24">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="V6" s="3" t="s">
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="V6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="X6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:24">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="V7" s="3" t="s">
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="V7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="W7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="X7" s="3" t="s">
+      <c r="X7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:24">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="V8" s="3" t="s">
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="V8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="W8" s="3" t="s">
+      <c r="W8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="X8" s="3" t="s">
+      <c r="X8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:24">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="V9" s="4" t="s">
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="V9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="W9" s="4" t="s">
+      <c r="W9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="X9" s="4" t="s">
+      <c r="X9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:24">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="V10" s="4" t="s">
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="V10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="W10" s="4" t="s">
+      <c r="W10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X10" s="4" t="s">
+      <c r="X10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:24">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="V11" s="4" t="s">
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="V11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="W11" s="4" t="s">
+      <c r="W11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X11" s="4" t="s">
+      <c r="X11" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="2:24">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="3"/>
+      <c r="F12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="H12" s="3"/>
+      <c r="J12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="N12" s="4" t="s">
+      <c r="L12" s="3"/>
+      <c r="N12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="V12" s="4" t="s">
+      <c r="P12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="V12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="W12" s="4" t="s">
+      <c r="W12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="X12" s="4"/>
+      <c r="X12" s="3"/>
     </row>
     <row r="13" spans="2:24">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="3"/>
+      <c r="F13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="J13" s="4" t="s">
+      <c r="H13" s="3"/>
+      <c r="J13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="N13" s="4" t="s">
+      <c r="L13" s="3"/>
+      <c r="N13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="P13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="V13" s="4" t="s">
+      <c r="P13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="V13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W13" s="4" t="s">
+      <c r="W13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X13" s="4"/>
+      <c r="X13" s="3"/>
     </row>
     <row r="14" spans="2:24">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="3"/>
+      <c r="F14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="J14" s="4" t="s">
+      <c r="H14" s="3"/>
+      <c r="J14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="N14" s="4" t="s">
+      <c r="L14" s="3"/>
+      <c r="N14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="V14" s="4" t="s">
+      <c r="P14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="V14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="W14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="X14" s="4"/>
+      <c r="X14" s="3"/>
     </row>
     <row r="15" spans="2:24">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="F15" s="4" t="s">
+      <c r="D15" s="3"/>
+      <c r="F15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="J15" s="4" t="s">
+      <c r="H15" s="3"/>
+      <c r="J15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="N15" s="4" t="s">
+      <c r="L15" s="3"/>
+      <c r="N15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="P15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="V15" s="4" t="s">
+      <c r="P15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="V15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="W15" s="4" t="s">
+      <c r="W15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X15" s="4"/>
+      <c r="X15" s="3"/>
     </row>
     <row r="16" spans="2:24">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="F16" s="5" t="s">
+      <c r="D16" s="4"/>
+      <c r="F16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="J16" s="5" t="s">
+      <c r="H16" s="4"/>
+      <c r="J16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="5"/>
-      <c r="N16" s="5" t="s">
+      <c r="L16" s="4"/>
+      <c r="N16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="O16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="V16" s="5" t="s">
+      <c r="P16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="V16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W16" s="5" t="s">
+      <c r="W16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X16" s="5"/>
+      <c r="X16" s="4"/>
     </row>
     <row r="17" spans="2:24">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="D17" s="4"/>
+      <c r="F17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="J17" s="5" t="s">
+      <c r="H17" s="4"/>
+      <c r="J17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="5"/>
-      <c r="N17" s="5" t="s">
+      <c r="L17" s="4"/>
+      <c r="N17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O17" s="5" t="s">
+      <c r="O17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="V17" s="5" t="s">
+      <c r="P17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="V17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="W17" s="5" t="s">
+      <c r="W17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="X17" s="5"/>
+      <c r="X17" s="4"/>
     </row>
     <row r="18" spans="2:24">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
     </row>
     <row r="19" spans="2:24">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
     </row>
     <row r="20" spans="2:24">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
     </row>
     <row r="21" spans="2:24">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
     </row>
     <row r="22" spans="2:24">
       <c r="B22" s="1"/>

</xml_diff>